<commit_message>
Task 3 finished, complete task 4 now
</commit_message>
<xml_diff>
--- a/Coursework/Data.xlsx
+++ b/Coursework/Data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40173513\Documents\Databases\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Advanced Databases\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Branch" sheetId="1" r:id="rId1"/>
@@ -441,9 +441,6 @@
     <t>01311112233</t>
   </si>
   <si>
-    <t>0781209888   0781209858    0781209840</t>
-  </si>
-  <si>
     <t>Cashier</t>
   </si>
   <si>
@@ -483,9 +480,6 @@
     <t>01311112277</t>
   </si>
   <si>
-    <t>0781209999   0781207865    0781209125</t>
-  </si>
-  <si>
     <t>Monica</t>
   </si>
   <si>
@@ -747,7 +741,13 @@
     <t>0770209999     0781207865      0781209125</t>
   </si>
   <si>
-    <t>0781209888     0781209858      0781209840</t>
+    <t>0770209888   0781209858    0781209840</t>
+  </si>
+  <si>
+    <t>0770209999   0781207865    0781209125</t>
+  </si>
+  <si>
+    <t>0770209888     0781209858      0781209840</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1707,7 @@
         <v>37453</v>
       </c>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="13">
         <v>1015</v>
       </c>
@@ -2084,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:M15"/>
+    <sheetView topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2321,7 @@
         <v>115</v>
       </c>
       <c r="N7" s="6">
-        <v>801</v>
+        <v>101</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>116</v>
@@ -2409,7 +2409,7 @@
         <v>136</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>137</v>
+        <v>237</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>120</v>
@@ -2447,16 +2447,16 @@
         <v>106</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="L10" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>121</v>
@@ -2497,13 +2497,13 @@
         <v>126</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K11" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="L11" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>122</v>
@@ -2541,16 +2541,16 @@
         <v>94</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="L12" s="11" t="s">
-        <v>151</v>
+        <v>238</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>123</v>
@@ -2588,16 +2588,16 @@
         <v>94</v>
       </c>
       <c r="I13" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="L13" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>124</v>
@@ -2635,19 +2635,19 @@
         <v>106</v>
       </c>
       <c r="I14" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="L14" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N14" s="6">
         <v>105</v>
@@ -2682,25 +2682,25 @@
         <v>94</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N15" s="6">
         <v>105</v>
       </c>
       <c r="O15" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P15" s="6">
         <v>25000</v>
@@ -2717,37 +2717,37 @@
         <v>117</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N16" s="6">
         <v>109</v>
       </c>
       <c r="O16" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P16" s="6">
         <v>25000</v>
@@ -2764,31 +2764,31 @@
         <v>118</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="N17" s="6">
         <v>109</v>
@@ -2811,37 +2811,37 @@
         <v>119</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N18" s="6">
         <v>109</v>
       </c>
       <c r="O18" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P18" s="6">
         <v>25000</v>
@@ -2858,29 +2858,29 @@
         <v>120</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N19" s="6">
         <v>111</v>
@@ -2903,37 +2903,37 @@
         <v>121</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N20" s="6">
         <v>111</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P20" s="6">
         <v>25000</v>
@@ -2950,37 +2950,37 @@
         <v>122</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N21" s="6">
         <v>111</v>
       </c>
       <c r="O21" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P21" s="6">
         <v>25000</v>
@@ -2997,37 +2997,37 @@
         <v>123</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N22" s="6">
         <v>110</v>
       </c>
       <c r="O22" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P22" s="6">
         <v>25000</v>
@@ -3044,31 +3044,31 @@
         <v>124</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H23" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="N23" s="6">
         <v>110</v>
@@ -3096,7 +3096,7 @@
   <dimension ref="D3:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23:M23"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,7 +3112,7 @@
   <sheetData>
     <row r="3" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>80</v>
@@ -3172,7 +3172,7 @@
         <v>131</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>115</v>
@@ -3192,10 +3192,10 @@
         <v>105</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>96</v>
@@ -3204,10 +3204,10 @@
         <v>131</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.25">
@@ -3221,23 +3221,23 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I6" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>223</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>225</v>
       </c>
       <c r="L6" s="11"/>
       <c r="M6" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="4:17" x14ac:dyDescent="0.25">
@@ -3245,29 +3245,29 @@
         <v>1004</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.25">
@@ -3275,31 +3275,31 @@
         <v>1005</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="4:17" ht="30" x14ac:dyDescent="0.25">
@@ -3307,31 +3307,31 @@
         <v>1006</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I9" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>232</v>
-      </c>
       <c r="M9" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.25">
@@ -3351,19 +3351,19 @@
         <v>106</v>
       </c>
       <c r="I10" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>157</v>
-      </c>
       <c r="L10" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="4:17" x14ac:dyDescent="0.25">
@@ -3380,22 +3380,22 @@
         <v>37</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I11" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="M11" s="6" t="s">
         <v>233</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="12" spans="4:17" x14ac:dyDescent="0.25">
@@ -3403,31 +3403,31 @@
         <v>1009</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="4:17" ht="45" x14ac:dyDescent="0.25">
@@ -3435,13 +3435,13 @@
         <v>1010</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>106</v>
@@ -3450,16 +3450,16 @@
         <v>107</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="4:17" x14ac:dyDescent="0.25">
@@ -3467,31 +3467,31 @@
         <v>1011</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="4:17" x14ac:dyDescent="0.25">
@@ -3499,31 +3499,31 @@
         <v>1012</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="L15" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="4:17" x14ac:dyDescent="0.25">
@@ -3531,31 +3531,31 @@
         <v>1013</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="4:13" ht="45" x14ac:dyDescent="0.25">
@@ -3575,16 +3575,16 @@
         <v>94</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="K17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="K17" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="L17" s="11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>123</v>
@@ -3639,16 +3639,16 @@
         <v>106</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="K19" s="9" t="s">
+      <c r="L19" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>121</v>
@@ -3674,13 +3674,13 @@
         <v>126</v>
       </c>
       <c r="J20" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K20" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="L20" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>122</v>
@@ -3691,31 +3691,31 @@
         <v>1018</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H21" s="6" t="s">
         <v>94</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="4:13" x14ac:dyDescent="0.25">
@@ -3723,31 +3723,31 @@
         <v>1019</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>106</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L22" s="11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M22" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="4:13" x14ac:dyDescent="0.25">
@@ -3767,23 +3767,24 @@
         <v>94</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3791,7 +3792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -3799,7 +3800,7 @@
   <sheetData>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Almost finished -Finish question 5 -Try to do more of the queries -Print it and fuck it
</commit_message>
<xml_diff>
--- a/Coursework/Data.xlsx
+++ b/Coursework/Data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Advanced Databases\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40173513\Documents\Databases\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Branch" sheetId="1" r:id="rId1"/>
@@ -738,16 +738,16 @@
     <t>0770123456       0770123489       0770125436</t>
   </si>
   <si>
-    <t>0770209999     0781207865      0781209125</t>
-  </si>
-  <si>
     <t>0770209888   0781209858    0781209840</t>
   </si>
   <si>
-    <t>0770209999   0781207865    0781209125</t>
-  </si>
-  <si>
     <t>0770209888     0781209858      0781209840</t>
+  </si>
+  <si>
+    <t>0790209999   0781207865    0781209125</t>
+  </si>
+  <si>
+    <t>0790209999      0781207865       0781209125</t>
   </si>
 </sst>
 </file>
@@ -1519,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2409,7 +2409,7 @@
         <v>136</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>120</v>
@@ -3096,7 +3096,7 @@
   <dimension ref="D3:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3584,7 +3584,7 @@
         <v>149</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>123</v>
@@ -3616,7 +3616,7 @@
         <v>136</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>120</v>
@@ -3792,7 +3792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>

</xml_diff>